<commit_message>
Se cambiaron los archivos del punto 3, 4 y 5
</commit_message>
<xml_diff>
--- a/Punto 5  Reporte issue.xlsx
+++ b/Punto 5  Reporte issue.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Reporte issue" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Copia de Reporte issue" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>Para  el tema de las ISSUES de acuerdo lo que se charle con el cliente el registro de las respectivas incidencias se podria hacer via correo, drive compartido por el cliente, o en alguna plataforma como JIRA o Azure Devops, en todo caso en cualquier escenario la issue se debe reportar y debe contener como minimo la siguiente infromacion:</t>
   </si>
@@ -19,10 +19,22 @@
     <t>REPORTE ISSUES</t>
   </si>
   <si>
+    <t>DIRIGIADO A.</t>
+  </si>
+  <si>
+    <t>Equipo desarollo</t>
+  </si>
+  <si>
+    <t>COPIA A:</t>
+  </si>
+  <si>
+    <t>Equipo Tester, PO, lider de proyecto</t>
+  </si>
+  <si>
     <t>NOMBRE ISSUE</t>
   </si>
   <si>
-    <t>Curso java sin imagen</t>
+    <t>Radicado : Curso java sin imagen</t>
   </si>
   <si>
     <t>Se le da un mombre a la incidencia</t>
@@ -31,8 +43,8 @@
     <t>DESCRIPCION GENERAL</t>
   </si>
   <si>
-    <t xml:space="preserve">Se evidencio que el curso de java no presenta la
- imagen </t>
+    <t xml:space="preserve">
+Se probo el aplicativo CHOUCAIR ACADEMY en el modulo Cursos y certificaciones en ambiente de calidad y se evidencio que al consultar el curso de Java este no presenta la imagen principal del curso</t>
   </si>
   <si>
     <t>Se hara un resumen de la prueba hecha y la no confomridad o hallazgo encontrado</t>
@@ -47,6 +59,12 @@
     <t>De acuerdo a la criticidad del evento se dara un status de: Alta-media.baja</t>
   </si>
   <si>
+    <t>AMBIENTE:</t>
+  </si>
+  <si>
+    <t>Calidad</t>
+  </si>
+  <si>
     <t>PLATAFOMA</t>
   </si>
   <si>
@@ -62,13 +80,19 @@
     <t>Cursos y Certificaciones</t>
   </si>
   <si>
-    <t xml:space="preserve">Adjuntos </t>
-  </si>
-  <si>
-    <t xml:space="preserve">imagen </t>
-  </si>
-  <si>
-    <t>Se envia una captura de pantalla donde se evidencia la falla</t>
+    <t>ESTADO:</t>
+  </si>
+  <si>
+    <t>Reportado</t>
+  </si>
+  <si>
+    <t>ADJUNTOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Imagen </t>
+  </si>
+  <si>
+    <t>Se adjunta imagen del error</t>
   </si>
   <si>
     <r>
@@ -119,15 +143,15 @@
     </font>
     <font>
       <b/>
+      <sz val="11.0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11.0"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="4">
@@ -252,7 +276,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -278,10 +302,13 @@
     <xf borderId="10" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="11" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="12" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="12" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf borderId="12" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="12" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
@@ -291,15 +318,12 @@
     </xf>
     <xf borderId="12" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -314,6 +338,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -324,7 +351,92 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="6334125" cy="3343275"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="0" name="image2.png" title="Imagen"/>
+        <xdr:cNvPicPr preferRelativeResize="0"/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5676900" cy="1647825"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="0" name="image3.png" title="Imagen"/>
+        <xdr:cNvPicPr preferRelativeResize="0"/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip cstate="print" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5638800" cy="1343025"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="0" name="image1.png" title="Imagen"/>
+        <xdr:cNvPicPr preferRelativeResize="0"/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip cstate="print" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -583,190 +695,209 @@
       <c r="C11" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="15" t="s">
-        <v>4</v>
-      </c>
+      <c r="D11" s="14"/>
     </row>
     <row r="12">
       <c r="B12" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="D12" s="14"/>
+    </row>
+    <row r="13">
+      <c r="B13" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="C13" s="14" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="13">
-      <c r="B13" s="14" t="s">
+      <c r="D13" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="14" t="s">
+    </row>
+    <row r="14" ht="90.0" customHeight="1">
+      <c r="B14" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="17" t="s">
+      <c r="C14" s="16" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="14">
-      <c r="B14" s="14" t="s">
+      <c r="D14" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="14" t="s">
+    </row>
+    <row r="15">
+      <c r="B15" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="17" t="s">
+      <c r="C15" s="15" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15">
-      <c r="B15" s="14" t="s">
+      <c r="D15" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="14" t="s">
+    </row>
+    <row r="16">
+      <c r="B16" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="B16" s="18" t="s">
+      <c r="C16" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="D16" s="18"/>
+    </row>
+    <row r="17">
+      <c r="B17" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="18" t="s">
+      <c r="C17" s="15" t="s">
         <v>18</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="19">
       <c r="B19" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" s="3"/>
-      <c r="D19" s="4"/>
+        <v>22</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="19"/>
     </row>
     <row r="20">
-      <c r="B20" s="6"/>
-      <c r="D20" s="7"/>
-    </row>
-    <row r="21">
-      <c r="B21" s="8"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="10"/>
-    </row>
-    <row r="28">
-      <c r="A28" s="20"/>
-      <c r="B28" s="20"/>
-      <c r="C28" s="20"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="20"/>
-      <c r="G28" s="20"/>
-      <c r="H28" s="20"/>
-    </row>
-    <row r="29">
-      <c r="A29" s="20"/>
-      <c r="B29" s="21"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="21"/>
-      <c r="G29" s="21"/>
-      <c r="H29" s="21"/>
-    </row>
-    <row r="30">
-      <c r="A30" s="20"/>
-      <c r="B30" s="21"/>
-      <c r="C30" s="21"/>
-      <c r="D30" s="22"/>
-      <c r="F30" s="21"/>
-      <c r="G30" s="21"/>
-      <c r="H30" s="23"/>
-    </row>
-    <row r="31">
-      <c r="A31" s="20"/>
-      <c r="B31" s="22"/>
-      <c r="C31" s="22"/>
-      <c r="D31" s="22"/>
-      <c r="E31" s="22"/>
-      <c r="F31" s="22"/>
-      <c r="G31" s="22"/>
-      <c r="H31" s="21"/>
+      <c r="B20" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="20"/>
-      <c r="B32" s="21"/>
-      <c r="C32" s="21"/>
-      <c r="D32" s="24"/>
-      <c r="E32" s="24"/>
-      <c r="F32" s="24"/>
-      <c r="G32" s="23"/>
-      <c r="H32" s="21"/>
+      <c r="B32" s="20"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="20"/>
     </row>
     <row r="33">
       <c r="A33" s="20"/>
-      <c r="B33" s="25"/>
-      <c r="C33" s="25"/>
-      <c r="D33" s="23"/>
-      <c r="E33" s="23"/>
-      <c r="F33" s="23"/>
-      <c r="G33" s="23"/>
+      <c r="B33" s="21"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="21"/>
       <c r="H33" s="21"/>
     </row>
     <row r="34">
-      <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="26"/>
-      <c r="E34" s="26"/>
-      <c r="F34" s="26"/>
-      <c r="G34" s="27"/>
-      <c r="H34" s="5"/>
+      <c r="A34" s="20"/>
+      <c r="B34" s="21"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="22"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="21"/>
+      <c r="H34" s="23"/>
     </row>
     <row r="35">
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="26"/>
-      <c r="E35" s="26"/>
-      <c r="F35" s="26"/>
-      <c r="G35" s="27"/>
-      <c r="H35" s="5"/>
+      <c r="A35" s="20"/>
+      <c r="B35" s="22"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="22"/>
+      <c r="G35" s="22"/>
+      <c r="H35" s="21"/>
     </row>
     <row r="36">
-      <c r="B36" s="5"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
-      <c r="F36" s="5"/>
-      <c r="G36" s="27"/>
-      <c r="H36" s="5"/>
+      <c r="A36" s="20"/>
+      <c r="B36" s="21"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="24"/>
+      <c r="E36" s="24"/>
+      <c r="F36" s="24"/>
+      <c r="G36" s="23"/>
+      <c r="H36" s="21"/>
     </row>
     <row r="37">
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
-      <c r="G37" s="5"/>
-      <c r="H37" s="5"/>
+      <c r="A37" s="20"/>
+      <c r="B37" s="25"/>
+      <c r="C37" s="25"/>
+      <c r="D37" s="23"/>
+      <c r="E37" s="23"/>
+      <c r="F37" s="23"/>
+      <c r="G37" s="23"/>
+      <c r="H37" s="21"/>
+    </row>
+    <row r="38">
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="26"/>
+      <c r="E38" s="26"/>
+      <c r="F38" s="26"/>
+      <c r="G38" s="27"/>
+      <c r="H38" s="5"/>
+    </row>
+    <row r="39">
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="26"/>
+      <c r="E39" s="26"/>
+      <c r="F39" s="26"/>
+      <c r="G39" s="27"/>
+      <c r="H39" s="5"/>
+    </row>
+    <row r="40">
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="27"/>
+      <c r="H40" s="5"/>
+    </row>
+    <row r="41">
+      <c r="B41" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="C41" s="3"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
+      <c r="H41" s="5"/>
     </row>
     <row r="42">
-      <c r="B42" s="27"/>
+      <c r="B42" s="6"/>
+      <c r="D42" s="7"/>
     </row>
     <row r="43">
-      <c r="B43" s="5"/>
-    </row>
-    <row r="44">
-      <c r="B44" s="5"/>
-    </row>
-    <row r="45">
-      <c r="B45" s="5"/>
+      <c r="B43" s="8"/>
+      <c r="C43" s="9"/>
+      <c r="D43" s="10"/>
     </row>
     <row r="46">
-      <c r="B46" s="5"/>
+      <c r="B46" s="27"/>
     </row>
     <row r="47">
       <c r="B47" s="5"/>
@@ -776,13 +907,16 @@
     </row>
     <row r="49">
       <c r="B49" s="5"/>
+    </row>
+    <row r="53">
+      <c r="B53" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="B5:D7"/>
     <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B19:D21"/>
-    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="B41:D43"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>